<commit_message>
Update the design and include supplementary scientists
</commit_message>
<xml_diff>
--- a/USAuthors/Data/Author.design-2-HA.xlsx
+++ b/USAuthors/Data/Author.design-2-HA.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juchi\Box Sync\Abdi_lab\RM3\Data sets\InPrep\InClassExamples\USAuthors\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452F9196-9E00-45EA-A658-F3C05A23F358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CDAC34-F055-4ADE-83FF-410D07AE9738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5685" windowWidth="38640" windowHeight="21390" xr2:uid="{8205C31E-2908-416D-B534-2ACEB3475067}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{8205C31E-2908-416D-B534-2ACEB3475067}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$235</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$235</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="286">
   <si>
     <t>Lincoln, Abraham</t>
   </si>
@@ -893,6 +893,12 @@
   </si>
   <si>
     <t>keep-balanced</t>
+  </si>
+  <si>
+    <t>(include 2 Churchill)</t>
+  </si>
+  <si>
+    <t>Supp-balanced</t>
   </si>
 </sst>
 </file>
@@ -975,7 +981,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ju-Chi" refreshedDate="44499.693459722221" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="235" xr:uid="{990B0AAC-C321-4DEF-BDD8-19A682493ACD}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:I1048576" sheet="Sheet1"/>
+    <worksheetSource ref="A1:J1048576" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="keepDiCA" numFmtId="0">
@@ -3389,7 +3395,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1C269342-6DD4-4976-A393-8FCB2F3530C3}" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1C269342-6DD4-4976-A393-8FCB2F3530C3}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -3803,10 +3809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4629592B-0E0F-485D-B1E6-ECE7C0C63CAD}">
-  <dimension ref="A1:J235"/>
+  <dimension ref="A1:K235"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="158" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3814,7 +3820,7 @@
     <col min="2" max="2" width="38.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>275</v>
       </c>
@@ -3834,19 +3840,22 @@
         <v>283</v>
       </c>
       <c r="G1" t="s">
+        <v>285</v>
+      </c>
+      <c r="H1" t="s">
         <v>234</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>235</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>236</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>33</v>
       </c>
@@ -3856,17 +3865,20 @@
       <c r="D2" t="s">
         <v>268</v>
       </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>242</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>169</v>
       </c>
@@ -3876,14 +3888,14 @@
       <c r="D3" t="s">
         <v>269</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>251</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>276</v>
       </c>
@@ -3896,14 +3908,14 @@
       <c r="D4" t="s">
         <v>267</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>242</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>276</v>
       </c>
@@ -3916,14 +3928,14 @@
       <c r="D5" t="s">
         <v>267</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>245</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>276</v>
       </c>
@@ -3936,14 +3948,14 @@
       <c r="D6" t="s">
         <v>267</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>245</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>60</v>
       </c>
@@ -3953,14 +3965,14 @@
       <c r="D7" t="s">
         <v>267</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>242</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>276</v>
       </c>
@@ -3973,14 +3985,14 @@
       <c r="D8" t="s">
         <v>267</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>242</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>276</v>
       </c>
@@ -3993,14 +4005,14 @@
       <c r="D9" t="s">
         <v>267</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>246</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>147</v>
       </c>
@@ -4010,17 +4022,17 @@
       <c r="D10" t="s">
         <v>267</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>252</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>247</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>276</v>
       </c>
@@ -4033,14 +4045,14 @@
       <c r="D11" t="s">
         <v>267</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>240</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>56</v>
       </c>
@@ -4050,14 +4062,14 @@
       <c r="D12" t="s">
         <v>267</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>246</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>276</v>
       </c>
@@ -4070,14 +4082,14 @@
       <c r="D13" t="s">
         <v>267</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>242</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>152</v>
       </c>
@@ -4087,14 +4099,14 @@
       <c r="D14" t="s">
         <v>267</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>248</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>276</v>
       </c>
@@ -4107,14 +4119,14 @@
       <c r="D15" t="s">
         <v>267</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>240</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>73</v>
       </c>
@@ -4124,17 +4136,17 @@
       <c r="D16" t="s">
         <v>267</v>
       </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
         <v>248</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>276</v>
       </c>
@@ -4147,14 +4159,14 @@
       <c r="D17" t="s">
         <v>267</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>242</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>276</v>
       </c>
@@ -4167,17 +4179,17 @@
       <c r="D18" t="s">
         <v>267</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>240</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>239</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>276</v>
       </c>
@@ -4190,17 +4202,17 @@
       <c r="D19" t="s">
         <v>267</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>240</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>239</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>276</v>
       </c>
@@ -4213,17 +4225,17 @@
       <c r="D20" t="s">
         <v>267</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>240</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>239</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>276</v>
       </c>
@@ -4236,14 +4248,14 @@
       <c r="D21" t="s">
         <v>267</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>240</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>276</v>
       </c>
@@ -4259,14 +4271,14 @@
       <c r="F22" t="b">
         <v>0</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>242</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>276</v>
       </c>
@@ -4279,14 +4291,14 @@
       <c r="D23" t="s">
         <v>267</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>252</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>276</v>
       </c>
@@ -4299,14 +4311,14 @@
       <c r="D24" t="s">
         <v>267</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>240</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>108</v>
       </c>
@@ -4319,14 +4331,14 @@
       <c r="F25" t="b">
         <v>0</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>251</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>276</v>
       </c>
@@ -4339,14 +4351,14 @@
       <c r="D26" t="s">
         <v>267</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>240</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>276</v>
       </c>
@@ -4359,14 +4371,14 @@
       <c r="D27" t="s">
         <v>267</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>245</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>276</v>
       </c>
@@ -4379,14 +4391,14 @@
       <c r="D28" t="s">
         <v>267</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>248</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>39</v>
       </c>
@@ -4399,14 +4411,14 @@
       <c r="F29" t="b">
         <v>0</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>242</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>276</v>
       </c>
@@ -4419,17 +4431,17 @@
       <c r="D30" t="s">
         <v>267</v>
       </c>
-      <c r="F30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
         <v>252</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>276</v>
       </c>
@@ -4442,14 +4454,14 @@
       <c r="D31" t="s">
         <v>267</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>242</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>276</v>
       </c>
@@ -4462,14 +4474,14 @@
       <c r="D32" t="s">
         <v>267</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>242</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>112</v>
       </c>
@@ -4479,17 +4491,17 @@
       <c r="D33" t="s">
         <v>267</v>
       </c>
-      <c r="F33" t="b">
-        <v>0</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
         <v>245</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>276</v>
       </c>
@@ -4502,17 +4514,17 @@
       <c r="D34" t="s">
         <v>267</v>
       </c>
-      <c r="F34" t="b">
-        <v>0</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
         <v>245</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>146</v>
       </c>
@@ -4525,14 +4537,14 @@
       <c r="F35" t="b">
         <v>0</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>242</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>5</v>
       </c>
@@ -4545,14 +4557,14 @@
       <c r="F36" t="b">
         <v>0</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>244</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>276</v>
       </c>
@@ -4565,14 +4577,14 @@
       <c r="D37" t="s">
         <v>267</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>240</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>77</v>
       </c>
@@ -4585,14 +4597,14 @@
       <c r="F38" t="b">
         <v>0</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>240</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>276</v>
       </c>
@@ -4605,14 +4617,14 @@
       <c r="D39" t="s">
         <v>267</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>240</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>141</v>
       </c>
@@ -4622,17 +4634,17 @@
       <c r="D40" t="s">
         <v>267</v>
       </c>
-      <c r="F40" t="b">
-        <v>0</v>
-      </c>
-      <c r="H40" t="s">
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" t="s">
         <v>245</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>276</v>
       </c>
@@ -4645,14 +4657,14 @@
       <c r="D41" t="s">
         <v>267</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>240</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>276</v>
       </c>
@@ -4665,14 +4677,14 @@
       <c r="D42" t="s">
         <v>267</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>246</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>218</v>
       </c>
@@ -4688,14 +4700,14 @@
       <c r="F43" t="b">
         <v>0</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>240</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>276</v>
       </c>
@@ -4708,14 +4720,14 @@
       <c r="D44" t="s">
         <v>267</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>240</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>276</v>
       </c>
@@ -4728,14 +4740,14 @@
       <c r="D45" t="s">
         <v>267</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>251</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>276</v>
       </c>
@@ -4748,14 +4760,14 @@
       <c r="D46" t="s">
         <v>267</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
         <v>251</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>217</v>
       </c>
@@ -4771,11 +4783,11 @@
       <c r="F47" t="b">
         <v>0</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>276</v>
       </c>
@@ -4791,14 +4803,14 @@
       <c r="F48" t="b">
         <v>0</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>240</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>276</v>
       </c>
@@ -4811,14 +4823,14 @@
       <c r="D49" t="s">
         <v>267</v>
       </c>
-      <c r="H49" t="s">
+      <c r="I49" t="s">
         <v>240</v>
       </c>
-      <c r="I49" t="s">
+      <c r="J49" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>172</v>
       </c>
@@ -4828,17 +4840,17 @@
       <c r="D50" t="s">
         <v>267</v>
       </c>
-      <c r="F50" t="b">
-        <v>0</v>
-      </c>
-      <c r="H50" t="s">
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" t="s">
         <v>248</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>276</v>
       </c>
@@ -4851,14 +4863,14 @@
       <c r="D51" t="s">
         <v>267</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
         <v>242</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>276</v>
       </c>
@@ -4871,14 +4883,14 @@
       <c r="D52" t="s">
         <v>267</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>240</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>276</v>
       </c>
@@ -4891,14 +4903,14 @@
       <c r="D53" t="s">
         <v>267</v>
       </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
         <v>240</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>276</v>
       </c>
@@ -4911,14 +4923,14 @@
       <c r="D54" t="s">
         <v>267</v>
       </c>
-      <c r="H54" t="s">
+      <c r="I54" t="s">
         <v>240</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>276</v>
       </c>
@@ -4931,14 +4943,14 @@
       <c r="D55" t="s">
         <v>267</v>
       </c>
-      <c r="H55" t="s">
+      <c r="I55" t="s">
         <v>240</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>276</v>
       </c>
@@ -4954,14 +4966,14 @@
       <c r="F56" t="b">
         <v>0</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>256</v>
       </c>
-      <c r="I56" t="s">
+      <c r="J56" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>276</v>
       </c>
@@ -4974,14 +4986,14 @@
       <c r="D57" t="s">
         <v>267</v>
       </c>
-      <c r="H57" t="s">
+      <c r="I57" t="s">
         <v>242</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>37</v>
       </c>
@@ -4994,14 +5006,14 @@
       <c r="F58" t="b">
         <v>0</v>
       </c>
-      <c r="H58" t="s">
+      <c r="I58" t="s">
         <v>246</v>
       </c>
-      <c r="I58" t="s">
+      <c r="J58" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>276</v>
       </c>
@@ -5014,14 +5026,14 @@
       <c r="D59" t="s">
         <v>267</v>
       </c>
-      <c r="H59" t="s">
+      <c r="I59" t="s">
         <v>253</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J59" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>139</v>
       </c>
@@ -5034,14 +5046,14 @@
       <c r="F60" t="b">
         <v>0</v>
       </c>
-      <c r="H60" t="s">
+      <c r="I60" t="s">
         <v>242</v>
       </c>
-      <c r="I60" t="s">
+      <c r="J60" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>276</v>
       </c>
@@ -5054,14 +5066,14 @@
       <c r="D61" t="s">
         <v>267</v>
       </c>
-      <c r="H61" t="s">
+      <c r="I61" t="s">
         <v>240</v>
       </c>
-      <c r="I61" t="s">
+      <c r="J61" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>276</v>
       </c>
@@ -5074,14 +5086,14 @@
       <c r="D62" t="s">
         <v>267</v>
       </c>
-      <c r="H62" t="s">
+      <c r="I62" t="s">
         <v>246</v>
       </c>
-      <c r="I62" t="s">
+      <c r="J62" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>97</v>
       </c>
@@ -5091,17 +5103,17 @@
       <c r="D63" t="s">
         <v>267</v>
       </c>
-      <c r="F63" t="b">
-        <v>0</v>
-      </c>
-      <c r="H63" t="s">
+      <c r="G63" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63" t="s">
         <v>252</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>101</v>
       </c>
@@ -5114,14 +5126,14 @@
       <c r="F64" t="b">
         <v>0</v>
       </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>240</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>276</v>
       </c>
@@ -5134,14 +5146,14 @@
       <c r="D65" t="s">
         <v>267</v>
       </c>
-      <c r="H65" t="s">
+      <c r="I65" t="s">
         <v>240</v>
       </c>
-      <c r="I65" t="s">
+      <c r="J65" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>276</v>
       </c>
@@ -5154,14 +5166,14 @@
       <c r="D66" t="s">
         <v>267</v>
       </c>
-      <c r="H66" t="s">
+      <c r="I66" t="s">
         <v>240</v>
       </c>
-      <c r="I66" t="s">
+      <c r="J66" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>276</v>
       </c>
@@ -5174,14 +5186,14 @@
       <c r="D67" t="s">
         <v>267</v>
       </c>
-      <c r="H67" t="s">
+      <c r="I67" t="s">
         <v>242</v>
       </c>
-      <c r="I67" t="s">
+      <c r="J67" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>216</v>
       </c>
@@ -5198,7 +5210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>227</v>
       </c>
@@ -5215,7 +5227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>192</v>
       </c>
@@ -5232,7 +5244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>91</v>
       </c>
@@ -5242,14 +5254,14 @@
       <c r="D71" t="s">
         <v>266</v>
       </c>
-      <c r="H71" t="s">
+      <c r="I71" t="s">
         <v>251</v>
       </c>
-      <c r="I71" t="s">
+      <c r="J71" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>276</v>
       </c>
@@ -5262,14 +5274,14 @@
       <c r="D72" t="s">
         <v>266</v>
       </c>
-      <c r="H72" t="s">
+      <c r="I72" t="s">
         <v>248</v>
       </c>
-      <c r="I72" t="s">
+      <c r="J72" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>276</v>
       </c>
@@ -5285,14 +5297,17 @@
       <c r="G73" t="b">
         <v>1</v>
       </c>
-      <c r="H73" t="s">
+      <c r="H73" t="b">
+        <v>1</v>
+      </c>
+      <c r="I73" t="s">
         <v>238</v>
       </c>
-      <c r="I73" t="s">
+      <c r="J73" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>276</v>
       </c>
@@ -5305,14 +5320,14 @@
       <c r="D74" t="s">
         <v>266</v>
       </c>
-      <c r="H74" t="s">
+      <c r="I74" t="s">
         <v>245</v>
       </c>
-      <c r="I74" t="s">
+      <c r="J74" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>194</v>
       </c>
@@ -5328,11 +5343,11 @@
       <c r="F75" t="b">
         <v>0</v>
       </c>
-      <c r="I75" t="s">
+      <c r="J75" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>119</v>
       </c>
@@ -5345,14 +5360,17 @@
       <c r="G76" t="b">
         <v>1</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H76" t="b">
+        <v>1</v>
+      </c>
+      <c r="I76" t="s">
         <v>238</v>
       </c>
-      <c r="I76" t="s">
+      <c r="J76" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>120</v>
       </c>
@@ -5365,14 +5383,17 @@
       <c r="G77" t="b">
         <v>1</v>
       </c>
-      <c r="H77" t="s">
+      <c r="H77" t="b">
+        <v>1</v>
+      </c>
+      <c r="I77" t="s">
         <v>238</v>
       </c>
-      <c r="I77" t="s">
+      <c r="J77" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>85</v>
       </c>
@@ -5382,14 +5403,14 @@
       <c r="D78" t="s">
         <v>266</v>
       </c>
-      <c r="H78" t="s">
+      <c r="I78" t="s">
         <v>252</v>
       </c>
-      <c r="I78" t="s">
+      <c r="J78" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>276</v>
       </c>
@@ -5402,14 +5423,14 @@
       <c r="D79" t="s">
         <v>266</v>
       </c>
-      <c r="H79" t="s">
+      <c r="I79" t="s">
         <v>240</v>
       </c>
-      <c r="I79" t="s">
+      <c r="J79" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>118</v>
       </c>
@@ -5422,14 +5443,17 @@
       <c r="G80" t="b">
         <v>1</v>
       </c>
-      <c r="H80" t="s">
+      <c r="H80" t="b">
+        <v>1</v>
+      </c>
+      <c r="I80" t="s">
         <v>238</v>
       </c>
-      <c r="I80" t="s">
+      <c r="J80" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>117</v>
       </c>
@@ -5442,14 +5466,17 @@
       <c r="G81" t="b">
         <v>1</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H81" t="b">
+        <v>1</v>
+      </c>
+      <c r="I81" t="s">
         <v>238</v>
       </c>
-      <c r="I81" t="s">
+      <c r="J81" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>276</v>
       </c>
@@ -5462,14 +5489,14 @@
       <c r="D82" t="s">
         <v>266</v>
       </c>
-      <c r="H82" t="s">
+      <c r="I82" t="s">
         <v>240</v>
       </c>
-      <c r="I82" t="s">
+      <c r="J82" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>276</v>
       </c>
@@ -5485,14 +5512,17 @@
       <c r="G83" t="b">
         <v>1</v>
       </c>
-      <c r="H83" t="s">
+      <c r="H83" t="b">
+        <v>1</v>
+      </c>
+      <c r="I83" t="s">
         <v>238</v>
       </c>
-      <c r="I83" t="s">
+      <c r="J83" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>121</v>
       </c>
@@ -5505,14 +5535,17 @@
       <c r="G84" t="b">
         <v>1</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I84" t="s">
         <v>238</v>
       </c>
-      <c r="I84" t="s">
+      <c r="J84" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>276</v>
       </c>
@@ -5525,14 +5558,14 @@
       <c r="D85" t="s">
         <v>266</v>
       </c>
-      <c r="H85" t="s">
+      <c r="I85" t="s">
         <v>240</v>
       </c>
-      <c r="I85" t="s">
+      <c r="J85" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>276</v>
       </c>
@@ -5545,17 +5578,20 @@
       <c r="D86" t="s">
         <v>266</v>
       </c>
-      <c r="H86" t="s">
+      <c r="G86" t="b">
+        <v>1</v>
+      </c>
+      <c r="I86" t="s">
         <v>240</v>
       </c>
-      <c r="I86" t="s">
+      <c r="J86" t="s">
         <v>239</v>
       </c>
-      <c r="J86" t="s">
+      <c r="K86" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>276</v>
       </c>
@@ -5568,14 +5604,14 @@
       <c r="D87" t="s">
         <v>266</v>
       </c>
-      <c r="H87" t="s">
+      <c r="I87" t="s">
         <v>245</v>
       </c>
-      <c r="I87" t="s">
+      <c r="J87" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>276</v>
       </c>
@@ -5588,14 +5624,14 @@
       <c r="D88" t="s">
         <v>266</v>
       </c>
-      <c r="H88" t="s">
+      <c r="I88" t="s">
         <v>249</v>
       </c>
-      <c r="I88" t="s">
+      <c r="J88" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>45</v>
       </c>
@@ -5605,17 +5641,17 @@
       <c r="D89" t="s">
         <v>266</v>
       </c>
-      <c r="F89" t="b">
-        <v>0</v>
-      </c>
-      <c r="H89" t="s">
+      <c r="G89" t="b">
+        <v>1</v>
+      </c>
+      <c r="I89" t="s">
         <v>252</v>
       </c>
-      <c r="I89" t="s">
+      <c r="J89" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>81</v>
       </c>
@@ -5625,14 +5661,14 @@
       <c r="D90" t="s">
         <v>266</v>
       </c>
-      <c r="H90" t="s">
+      <c r="I90" t="s">
         <v>253</v>
       </c>
-      <c r="I90" t="s">
+      <c r="J90" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>276</v>
       </c>
@@ -5645,14 +5681,14 @@
       <c r="D91" t="s">
         <v>266</v>
       </c>
-      <c r="H91" t="s">
+      <c r="I91" t="s">
         <v>240</v>
       </c>
-      <c r="I91" t="s">
+      <c r="J91" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>104</v>
       </c>
@@ -5662,17 +5698,17 @@
       <c r="D92" t="s">
         <v>266</v>
       </c>
-      <c r="F92" t="b">
-        <v>0</v>
-      </c>
-      <c r="H92" t="s">
+      <c r="G92" t="b">
+        <v>1</v>
+      </c>
+      <c r="I92" t="s">
         <v>252</v>
       </c>
-      <c r="I92" t="s">
+      <c r="J92" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>131</v>
       </c>
@@ -5685,14 +5721,17 @@
       <c r="G93" t="b">
         <v>1</v>
       </c>
-      <c r="H93" t="s">
+      <c r="H93" t="b">
+        <v>1</v>
+      </c>
+      <c r="I93" t="s">
         <v>238</v>
       </c>
-      <c r="I93" t="s">
+      <c r="J93" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>129</v>
       </c>
@@ -5705,14 +5744,17 @@
       <c r="G94" t="b">
         <v>1</v>
       </c>
-      <c r="H94" t="s">
+      <c r="H94" t="b">
+        <v>1</v>
+      </c>
+      <c r="I94" t="s">
         <v>238</v>
       </c>
-      <c r="I94" t="s">
+      <c r="J94" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>122</v>
       </c>
@@ -5725,14 +5767,17 @@
       <c r="G95" t="b">
         <v>1</v>
       </c>
-      <c r="H95" t="s">
+      <c r="H95" t="b">
+        <v>1</v>
+      </c>
+      <c r="I95" t="s">
         <v>238</v>
       </c>
-      <c r="I95" t="s">
+      <c r="J95" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>276</v>
       </c>
@@ -5745,14 +5790,14 @@
       <c r="D96" t="s">
         <v>266</v>
       </c>
-      <c r="H96" t="s">
+      <c r="I96" t="s">
         <v>240</v>
       </c>
-      <c r="I96" t="s">
+      <c r="J96" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>125</v>
       </c>
@@ -5765,14 +5810,17 @@
       <c r="G97" t="b">
         <v>1</v>
       </c>
-      <c r="H97" t="s">
+      <c r="H97" t="b">
+        <v>1</v>
+      </c>
+      <c r="I97" t="s">
         <v>238</v>
       </c>
-      <c r="I97" t="s">
+      <c r="J97" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>276</v>
       </c>
@@ -5785,14 +5833,14 @@
       <c r="D98" t="s">
         <v>266</v>
       </c>
-      <c r="H98" t="s">
+      <c r="I98" t="s">
         <v>242</v>
       </c>
-      <c r="I98" t="s">
+      <c r="J98" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>276</v>
       </c>
@@ -5805,14 +5853,14 @@
       <c r="D99" t="s">
         <v>266</v>
       </c>
-      <c r="H99" t="s">
+      <c r="I99" t="s">
         <v>240</v>
       </c>
-      <c r="I99" t="s">
+      <c r="J99" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>162</v>
       </c>
@@ -5825,14 +5873,14 @@
       <c r="F100" t="b">
         <v>0</v>
       </c>
-      <c r="H100" t="s">
+      <c r="I100" t="s">
         <v>242</v>
       </c>
-      <c r="I100" t="s">
+      <c r="J100" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>276</v>
       </c>
@@ -5845,14 +5893,14 @@
       <c r="D101" t="s">
         <v>266</v>
       </c>
-      <c r="H101" t="s">
+      <c r="I101" t="s">
         <v>242</v>
       </c>
-      <c r="I101" t="s">
+      <c r="J101" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>123</v>
       </c>
@@ -5865,14 +5913,17 @@
       <c r="G102" t="b">
         <v>1</v>
       </c>
-      <c r="H102" t="s">
+      <c r="H102" t="b">
+        <v>1</v>
+      </c>
+      <c r="I102" t="s">
         <v>238</v>
       </c>
-      <c r="I102" t="s">
+      <c r="J102" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>107</v>
       </c>
@@ -5885,14 +5936,14 @@
       <c r="F103" t="b">
         <v>0</v>
       </c>
-      <c r="H103" t="s">
+      <c r="I103" t="s">
         <v>258</v>
       </c>
-      <c r="I103" t="s">
+      <c r="J103" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>276</v>
       </c>
@@ -5905,14 +5956,14 @@
       <c r="D104" t="s">
         <v>266</v>
       </c>
-      <c r="H104" t="s">
+      <c r="I104" t="s">
         <v>248</v>
       </c>
-      <c r="I104" t="s">
+      <c r="J104" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>127</v>
       </c>
@@ -5925,14 +5976,17 @@
       <c r="G105" t="b">
         <v>1</v>
       </c>
-      <c r="H105" t="s">
+      <c r="H105" t="b">
+        <v>1</v>
+      </c>
+      <c r="I105" t="s">
         <v>238</v>
       </c>
-      <c r="I105" t="s">
+      <c r="J105" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>80</v>
       </c>
@@ -5942,14 +5996,14 @@
       <c r="D106" t="s">
         <v>266</v>
       </c>
-      <c r="H106" t="s">
+      <c r="I106" t="s">
         <v>240</v>
       </c>
-      <c r="I106" t="s">
+      <c r="J106" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>126</v>
       </c>
@@ -5962,14 +6016,17 @@
       <c r="G107" t="b">
         <v>1</v>
       </c>
-      <c r="H107" t="s">
+      <c r="H107" t="b">
+        <v>1</v>
+      </c>
+      <c r="I107" t="s">
         <v>238</v>
       </c>
-      <c r="I107" t="s">
+      <c r="J107" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>276</v>
       </c>
@@ -5982,14 +6039,14 @@
       <c r="D108" t="s">
         <v>266</v>
       </c>
-      <c r="H108" t="s">
+      <c r="I108" t="s">
         <v>240</v>
       </c>
-      <c r="I108" t="s">
+      <c r="J108" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>276</v>
       </c>
@@ -6002,14 +6059,14 @@
       <c r="D109" t="s">
         <v>266</v>
       </c>
-      <c r="H109" t="s">
+      <c r="I109" t="s">
         <v>240</v>
       </c>
-      <c r="I109" t="s">
+      <c r="J109" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>44</v>
       </c>
@@ -6022,14 +6079,14 @@
       <c r="F110" t="b">
         <v>0</v>
       </c>
-      <c r="H110" t="s">
+      <c r="I110" t="s">
         <v>251</v>
       </c>
-      <c r="I110" t="s">
+      <c r="J110" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
         <v>128</v>
       </c>
@@ -6042,14 +6099,17 @@
       <c r="G111" t="b">
         <v>1</v>
       </c>
-      <c r="H111" t="s">
+      <c r="H111" t="b">
+        <v>1</v>
+      </c>
+      <c r="I111" t="s">
         <v>238</v>
       </c>
-      <c r="I111" t="s">
+      <c r="J111" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>130</v>
       </c>
@@ -6062,14 +6122,17 @@
       <c r="G112" t="b">
         <v>1</v>
       </c>
-      <c r="H112" t="s">
+      <c r="H112" t="b">
+        <v>1</v>
+      </c>
+      <c r="I112" t="s">
         <v>238</v>
       </c>
-      <c r="I112" t="s">
+      <c r="J112" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>84</v>
       </c>
@@ -6082,14 +6145,14 @@
       <c r="F113" t="b">
         <v>0</v>
       </c>
-      <c r="H113" t="s">
+      <c r="I113" t="s">
         <v>240</v>
       </c>
-      <c r="I113" t="s">
+      <c r="J113" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>191</v>
       </c>
@@ -6105,14 +6168,14 @@
       <c r="F114" t="b">
         <v>0</v>
       </c>
-      <c r="H114" t="s">
+      <c r="I114" t="s">
         <v>256</v>
       </c>
-      <c r="I114" t="s">
+      <c r="J114" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>153</v>
       </c>
@@ -6122,14 +6185,14 @@
       <c r="D115" t="s">
         <v>266</v>
       </c>
-      <c r="H115" t="s">
+      <c r="I115" t="s">
         <v>248</v>
       </c>
-      <c r="I115" t="s">
+      <c r="J115" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
         <v>136</v>
       </c>
@@ -6139,14 +6202,14 @@
       <c r="D116" t="s">
         <v>266</v>
       </c>
-      <c r="H116" t="s">
+      <c r="I116" t="s">
         <v>240</v>
       </c>
-      <c r="I116" t="s">
+      <c r="J116" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>124</v>
       </c>
@@ -6159,14 +6222,17 @@
       <c r="G117" t="b">
         <v>1</v>
       </c>
-      <c r="H117" t="s">
+      <c r="H117" t="b">
+        <v>1</v>
+      </c>
+      <c r="I117" t="s">
         <v>238</v>
       </c>
-      <c r="I117" t="s">
+      <c r="J117" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>276</v>
       </c>
@@ -6179,14 +6245,14 @@
       <c r="D118" t="s">
         <v>266</v>
       </c>
-      <c r="H118" t="s">
+      <c r="I118" t="s">
         <v>240</v>
       </c>
-      <c r="I118" t="s">
+      <c r="J118" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>182</v>
       </c>
@@ -6202,14 +6268,14 @@
       <c r="F119" t="b">
         <v>0</v>
       </c>
-      <c r="H119" t="s">
+      <c r="I119" t="s">
         <v>240</v>
       </c>
-      <c r="I119" t="s">
+      <c r="J119" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>29</v>
       </c>
@@ -6222,14 +6288,14 @@
       <c r="F120" t="b">
         <v>0</v>
       </c>
-      <c r="H120" t="s">
+      <c r="I120" t="s">
         <v>240</v>
       </c>
-      <c r="I120" t="s">
+      <c r="J120" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
         <v>133</v>
       </c>
@@ -6242,14 +6308,17 @@
       <c r="G121" t="b">
         <v>1</v>
       </c>
-      <c r="H121" t="s">
+      <c r="H121" t="b">
+        <v>1</v>
+      </c>
+      <c r="I121" t="s">
         <v>238</v>
       </c>
-      <c r="I121" t="s">
+      <c r="J121" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>276</v>
       </c>
@@ -6262,14 +6331,14 @@
       <c r="D122" t="s">
         <v>266</v>
       </c>
-      <c r="H122" t="s">
+      <c r="I122" t="s">
         <v>240</v>
       </c>
-      <c r="I122" t="s">
+      <c r="J122" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B123" t="s">
         <v>132</v>
       </c>
@@ -6282,14 +6351,17 @@
       <c r="G123" t="b">
         <v>1</v>
       </c>
-      <c r="H123" t="s">
+      <c r="H123" t="b">
+        <v>1</v>
+      </c>
+      <c r="I123" t="s">
         <v>238</v>
       </c>
-      <c r="I123" t="s">
+      <c r="J123" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
         <v>148</v>
       </c>
@@ -6302,14 +6374,17 @@
       <c r="G124" t="b">
         <v>1</v>
       </c>
-      <c r="H124" t="s">
+      <c r="H124" t="b">
+        <v>1</v>
+      </c>
+      <c r="I124" t="s">
         <v>238</v>
       </c>
-      <c r="I124" t="s">
+      <c r="J124" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>276</v>
       </c>
@@ -6322,14 +6397,14 @@
       <c r="D125" t="s">
         <v>266</v>
       </c>
-      <c r="H125" t="s">
+      <c r="I125" t="s">
         <v>263</v>
       </c>
-      <c r="I125" t="s">
+      <c r="J125" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
         <v>219</v>
       </c>
@@ -6343,7 +6418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>276</v>
       </c>
@@ -6356,14 +6431,14 @@
       <c r="D127" t="s">
         <v>266</v>
       </c>
-      <c r="H127" t="s">
+      <c r="I127" t="s">
         <v>240</v>
       </c>
-      <c r="I127" t="s">
+      <c r="J127" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
         <v>185</v>
       </c>
@@ -6377,7 +6452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>276</v>
       </c>
@@ -6390,14 +6465,14 @@
       <c r="D129" t="s">
         <v>266</v>
       </c>
-      <c r="H129" t="s">
+      <c r="I129" t="s">
         <v>240</v>
       </c>
-      <c r="I129" t="s">
+      <c r="J129" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B130" t="s">
         <v>209</v>
       </c>
@@ -6410,11 +6485,11 @@
       <c r="F130" t="b">
         <v>0</v>
       </c>
-      <c r="J130" t="s">
+      <c r="K130" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B131" t="s">
         <v>178</v>
       </c>
@@ -6428,7 +6503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B132" t="s">
         <v>179</v>
       </c>
@@ -6442,7 +6517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B133" t="s">
         <v>221</v>
       </c>
@@ -6456,7 +6531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B134" t="s">
         <v>206</v>
       </c>
@@ -6470,7 +6545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B135" t="s">
         <v>229</v>
       </c>
@@ -6484,7 +6559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B136" t="s">
         <v>187</v>
       </c>
@@ -6498,7 +6573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
         <v>205</v>
       </c>
@@ -6512,7 +6587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B138" t="s">
         <v>193</v>
       </c>
@@ -6526,7 +6601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B139" t="s">
         <v>190</v>
       </c>
@@ -6540,7 +6615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B140" t="s">
         <v>210</v>
       </c>
@@ -6554,7 +6629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B141" t="s">
         <v>230</v>
       </c>
@@ -6568,7 +6643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B142" t="s">
         <v>106</v>
       </c>
@@ -6578,14 +6653,14 @@
       <c r="D142" t="s">
         <v>264</v>
       </c>
-      <c r="H142" t="s">
+      <c r="I142" t="s">
         <v>245</v>
       </c>
-      <c r="I142" t="s">
+      <c r="J142" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B143" t="s">
         <v>98</v>
       </c>
@@ -6595,14 +6670,14 @@
       <c r="D143" t="s">
         <v>264</v>
       </c>
-      <c r="H143" t="s">
+      <c r="I143" t="s">
         <v>246</v>
       </c>
-      <c r="I143" t="s">
+      <c r="J143" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B144" t="s">
         <v>10</v>
       </c>
@@ -6612,14 +6687,14 @@
       <c r="D144" t="s">
         <v>264</v>
       </c>
-      <c r="H144" t="s">
+      <c r="I144" t="s">
         <v>245</v>
       </c>
-      <c r="I144" t="s">
+      <c r="J144" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="145" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B145" t="s">
         <v>159</v>
       </c>
@@ -6629,14 +6704,14 @@
       <c r="D145" t="s">
         <v>264</v>
       </c>
-      <c r="H145" t="s">
+      <c r="I145" t="s">
         <v>256</v>
       </c>
-      <c r="I145" t="s">
+      <c r="J145" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B146" t="s">
         <v>49</v>
       </c>
@@ -6646,14 +6721,14 @@
       <c r="D146" t="s">
         <v>264</v>
       </c>
-      <c r="H146" t="s">
+      <c r="I146" t="s">
         <v>240</v>
       </c>
-      <c r="I146" t="s">
+      <c r="J146" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="147" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B147" t="s">
         <v>137</v>
       </c>
@@ -6663,14 +6738,14 @@
       <c r="D147" t="s">
         <v>264</v>
       </c>
-      <c r="H147" t="s">
+      <c r="I147" t="s">
         <v>242</v>
       </c>
-      <c r="I147" t="s">
+      <c r="J147" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="148" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B148" t="s">
         <v>90</v>
       </c>
@@ -6680,14 +6755,14 @@
       <c r="D148" t="s">
         <v>264</v>
       </c>
-      <c r="H148" t="s">
+      <c r="I148" t="s">
         <v>246</v>
       </c>
-      <c r="I148" t="s">
+      <c r="J148" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="149" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B149" t="s">
         <v>87</v>
       </c>
@@ -6697,14 +6772,14 @@
       <c r="D149" t="s">
         <v>264</v>
       </c>
-      <c r="H149" t="s">
+      <c r="I149" t="s">
         <v>246</v>
       </c>
-      <c r="I149" t="s">
+      <c r="J149" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B150" t="s">
         <v>173</v>
       </c>
@@ -6714,14 +6789,14 @@
       <c r="D150" t="s">
         <v>264</v>
       </c>
-      <c r="H150" t="s">
+      <c r="I150" t="s">
         <v>240</v>
       </c>
-      <c r="I150" t="s">
+      <c r="J150" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="151" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B151" t="s">
         <v>134</v>
       </c>
@@ -6731,14 +6806,14 @@
       <c r="D151" t="s">
         <v>264</v>
       </c>
-      <c r="H151" t="s">
+      <c r="I151" t="s">
         <v>242</v>
       </c>
-      <c r="I151" t="s">
+      <c r="J151" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="152" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B152" t="s">
         <v>144</v>
       </c>
@@ -6748,14 +6823,14 @@
       <c r="D152" t="s">
         <v>264</v>
       </c>
-      <c r="H152" t="s">
+      <c r="I152" t="s">
         <v>245</v>
       </c>
-      <c r="I152" t="s">
+      <c r="J152" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="153" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B153" t="s">
         <v>166</v>
       </c>
@@ -6765,14 +6840,14 @@
       <c r="D153" t="s">
         <v>264</v>
       </c>
-      <c r="H153" t="s">
+      <c r="I153" t="s">
         <v>245</v>
       </c>
-      <c r="I153" t="s">
+      <c r="J153" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="154" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B154" t="s">
         <v>50</v>
       </c>
@@ -6782,14 +6857,14 @@
       <c r="D154" t="s">
         <v>264</v>
       </c>
-      <c r="H154" t="s">
+      <c r="I154" t="s">
         <v>240</v>
       </c>
-      <c r="I154" t="s">
+      <c r="J154" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="155" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B155" t="s">
         <v>168</v>
       </c>
@@ -6799,14 +6874,14 @@
       <c r="D155" t="s">
         <v>264</v>
       </c>
-      <c r="H155" t="s">
+      <c r="I155" t="s">
         <v>251</v>
       </c>
-      <c r="I155" t="s">
+      <c r="J155" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="156" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B156" t="s">
         <v>94</v>
       </c>
@@ -6816,14 +6891,14 @@
       <c r="D156" t="s">
         <v>264</v>
       </c>
-      <c r="H156" t="s">
+      <c r="I156" t="s">
         <v>240</v>
       </c>
-      <c r="I156" t="s">
+      <c r="J156" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="157" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B157" t="s">
         <v>176</v>
       </c>
@@ -6836,14 +6911,14 @@
       <c r="F157" t="b">
         <v>0</v>
       </c>
-      <c r="H157" t="s">
+      <c r="I157" t="s">
         <v>240</v>
       </c>
-      <c r="I157" t="s">
+      <c r="J157" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="158" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B158" t="s">
         <v>51</v>
       </c>
@@ -6853,14 +6928,14 @@
       <c r="D158" t="s">
         <v>264</v>
       </c>
-      <c r="H158" t="s">
+      <c r="I158" t="s">
         <v>240</v>
       </c>
-      <c r="I158" t="s">
+      <c r="J158" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="159" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B159" t="s">
         <v>155</v>
       </c>
@@ -6873,14 +6948,14 @@
       <c r="F159" t="b">
         <v>0</v>
       </c>
-      <c r="H159" t="s">
+      <c r="I159" t="s">
         <v>240</v>
       </c>
-      <c r="I159" t="s">
+      <c r="J159" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="160" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B160" t="s">
         <v>142</v>
       </c>
@@ -6890,14 +6965,14 @@
       <c r="D160" t="s">
         <v>264</v>
       </c>
-      <c r="H160" t="s">
+      <c r="I160" t="s">
         <v>242</v>
       </c>
-      <c r="I160" t="s">
+      <c r="J160" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="161" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B161" t="s">
         <v>138</v>
       </c>
@@ -6907,17 +6982,17 @@
       <c r="D161" t="s">
         <v>264</v>
       </c>
-      <c r="F161" t="b">
-        <v>0</v>
-      </c>
-      <c r="H161" t="s">
+      <c r="G161" t="b">
+        <v>1</v>
+      </c>
+      <c r="I161" t="s">
         <v>248</v>
       </c>
-      <c r="I161" t="s">
+      <c r="J161" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="162" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B162" t="s">
         <v>149</v>
       </c>
@@ -6927,17 +7002,17 @@
       <c r="D162" t="s">
         <v>264</v>
       </c>
-      <c r="F162" t="b">
-        <v>0</v>
-      </c>
-      <c r="H162" t="s">
+      <c r="G162" t="b">
+        <v>1</v>
+      </c>
+      <c r="I162" t="s">
         <v>248</v>
       </c>
-      <c r="I162" t="s">
+      <c r="J162" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="163" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B163" t="s">
         <v>174</v>
       </c>
@@ -6950,14 +7025,14 @@
       <c r="F163" t="b">
         <v>0</v>
       </c>
-      <c r="H163" t="s">
+      <c r="I163" t="s">
         <v>251</v>
       </c>
-      <c r="I163" t="s">
+      <c r="J163" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="164" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B164" t="s">
         <v>82</v>
       </c>
@@ -6967,14 +7042,14 @@
       <c r="D164" t="s">
         <v>264</v>
       </c>
-      <c r="H164" t="s">
+      <c r="I164" t="s">
         <v>240</v>
       </c>
-      <c r="I164" t="s">
+      <c r="J164" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="165" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B165" t="s">
         <v>71</v>
       </c>
@@ -6984,14 +7059,14 @@
       <c r="D165" t="s">
         <v>264</v>
       </c>
-      <c r="H165" t="s">
+      <c r="I165" t="s">
         <v>240</v>
       </c>
-      <c r="I165" t="s">
+      <c r="J165" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="166" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B166" t="s">
         <v>74</v>
       </c>
@@ -7001,14 +7076,14 @@
       <c r="D166" t="s">
         <v>264</v>
       </c>
-      <c r="H166" t="s">
+      <c r="I166" t="s">
         <v>240</v>
       </c>
-      <c r="I166" t="s">
+      <c r="J166" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="167" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B167" t="s">
         <v>156</v>
       </c>
@@ -7018,14 +7093,14 @@
       <c r="D167" t="s">
         <v>264</v>
       </c>
-      <c r="H167" t="s">
+      <c r="I167" t="s">
         <v>242</v>
       </c>
-      <c r="I167" t="s">
+      <c r="J167" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="168" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B168" t="s">
         <v>167</v>
       </c>
@@ -7038,14 +7113,14 @@
       <c r="F168" t="b">
         <v>0</v>
       </c>
-      <c r="H168" t="s">
+      <c r="I168" t="s">
         <v>258</v>
       </c>
-      <c r="I168" t="s">
+      <c r="J168" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="169" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B169" t="s">
         <v>23</v>
       </c>
@@ -7055,14 +7130,14 @@
       <c r="D169" t="s">
         <v>264</v>
       </c>
-      <c r="H169" t="s">
+      <c r="I169" t="s">
         <v>240</v>
       </c>
-      <c r="I169" t="s">
+      <c r="J169" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="170" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B170" t="s">
         <v>164</v>
       </c>
@@ -7072,17 +7147,17 @@
       <c r="D170" t="s">
         <v>264</v>
       </c>
-      <c r="F170" t="b">
-        <v>0</v>
-      </c>
-      <c r="H170" t="s">
+      <c r="G170" t="b">
+        <v>1</v>
+      </c>
+      <c r="I170" t="s">
         <v>248</v>
       </c>
-      <c r="I170" t="s">
+      <c r="J170" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="171" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B171" t="s">
         <v>115</v>
       </c>
@@ -7095,14 +7170,14 @@
       <c r="F171" t="b">
         <v>0</v>
       </c>
-      <c r="H171" t="s">
+      <c r="I171" t="s">
         <v>249</v>
       </c>
-      <c r="I171" t="s">
+      <c r="J171" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="172" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B172" t="s">
         <v>57</v>
       </c>
@@ -7112,14 +7187,14 @@
       <c r="D172" t="s">
         <v>264</v>
       </c>
-      <c r="H172" t="s">
+      <c r="I172" t="s">
         <v>240</v>
       </c>
-      <c r="I172" t="s">
+      <c r="J172" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="173" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B173" t="s">
         <v>95</v>
       </c>
@@ -7129,14 +7204,14 @@
       <c r="D173" t="s">
         <v>264</v>
       </c>
-      <c r="H173" t="s">
+      <c r="I173" t="s">
         <v>240</v>
       </c>
-      <c r="I173" t="s">
+      <c r="J173" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="174" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B174" t="s">
         <v>161</v>
       </c>
@@ -7146,17 +7221,17 @@
       <c r="D174" t="s">
         <v>264</v>
       </c>
-      <c r="F174" t="b">
-        <v>0</v>
-      </c>
-      <c r="H174" t="s">
+      <c r="G174" t="b">
+        <v>1</v>
+      </c>
+      <c r="I174" t="s">
         <v>248</v>
       </c>
-      <c r="I174" t="s">
+      <c r="J174" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="175" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B175" t="s">
         <v>109</v>
       </c>
@@ -7166,14 +7241,14 @@
       <c r="D175" t="s">
         <v>264</v>
       </c>
-      <c r="H175" t="s">
+      <c r="I175" t="s">
         <v>246</v>
       </c>
-      <c r="I175" t="s">
+      <c r="J175" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="176" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B176" t="s">
         <v>92</v>
       </c>
@@ -7183,14 +7258,14 @@
       <c r="D176" t="s">
         <v>264</v>
       </c>
-      <c r="H176" t="s">
+      <c r="I176" t="s">
         <v>240</v>
       </c>
-      <c r="I176" t="s">
+      <c r="J176" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B177" t="s">
         <v>64</v>
       </c>
@@ -7200,14 +7275,14 @@
       <c r="D177" t="s">
         <v>264</v>
       </c>
-      <c r="H177" t="s">
+      <c r="I177" t="s">
         <v>240</v>
       </c>
-      <c r="I177" t="s">
+      <c r="J177" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="178" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B178" t="s">
         <v>99</v>
       </c>
@@ -7220,14 +7295,14 @@
       <c r="F178" t="b">
         <v>0</v>
       </c>
-      <c r="H178" t="s">
+      <c r="I178" t="s">
         <v>256</v>
       </c>
-      <c r="I178" t="s">
+      <c r="J178" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="179" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B179" t="s">
         <v>163</v>
       </c>
@@ -7240,14 +7315,14 @@
       <c r="F179" t="b">
         <v>0</v>
       </c>
-      <c r="H179" t="s">
+      <c r="I179" t="s">
         <v>251</v>
       </c>
-      <c r="I179" t="s">
+      <c r="J179" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B180" t="s">
         <v>66</v>
       </c>
@@ -7257,17 +7332,17 @@
       <c r="D180" t="s">
         <v>264</v>
       </c>
-      <c r="F180" t="b">
-        <v>0</v>
-      </c>
-      <c r="H180" t="s">
+      <c r="G180" t="b">
+        <v>1</v>
+      </c>
+      <c r="I180" t="s">
         <v>245</v>
       </c>
-      <c r="I180" t="s">
+      <c r="J180" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="181" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B181" t="s">
         <v>158</v>
       </c>
@@ -7280,14 +7355,14 @@
       <c r="F181" t="b">
         <v>0</v>
       </c>
-      <c r="H181" t="s">
+      <c r="I181" t="s">
         <v>256</v>
       </c>
-      <c r="I181" t="s">
+      <c r="J181" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B182" t="s">
         <v>114</v>
       </c>
@@ -7297,14 +7372,14 @@
       <c r="D182" t="s">
         <v>264</v>
       </c>
-      <c r="H182" t="s">
+      <c r="I182" t="s">
         <v>242</v>
       </c>
-      <c r="I182" t="s">
+      <c r="J182" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="183" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B183" t="s">
         <v>18</v>
       </c>
@@ -7314,14 +7389,14 @@
       <c r="D183" t="s">
         <v>264</v>
       </c>
-      <c r="H183" t="s">
+      <c r="I183" t="s">
         <v>240</v>
       </c>
-      <c r="I183" t="s">
+      <c r="J183" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="184" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B184" t="s">
         <v>110</v>
       </c>
@@ -7334,14 +7409,14 @@
       <c r="F184" t="b">
         <v>0</v>
       </c>
-      <c r="H184" t="s">
+      <c r="I184" t="s">
         <v>242</v>
       </c>
-      <c r="I184" t="s">
+      <c r="J184" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B185" t="s">
         <v>224</v>
       </c>
@@ -7357,14 +7432,14 @@
       <c r="F185" t="b">
         <v>0</v>
       </c>
-      <c r="H185" t="s">
+      <c r="I185" t="s">
         <v>248</v>
       </c>
-      <c r="I185" t="s">
+      <c r="J185" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="186" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B186" t="s">
         <v>72</v>
       </c>
@@ -7374,14 +7449,14 @@
       <c r="D186" t="s">
         <v>264</v>
       </c>
-      <c r="H186" t="s">
+      <c r="I186" t="s">
         <v>240</v>
       </c>
-      <c r="I186" t="s">
+      <c r="J186" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B187" t="s">
         <v>1</v>
       </c>
@@ -7394,14 +7469,14 @@
       <c r="F187" t="b">
         <v>0</v>
       </c>
-      <c r="H187" t="s">
+      <c r="I187" t="s">
         <v>240</v>
       </c>
-      <c r="I187" t="s">
+      <c r="J187" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="188" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B188" t="s">
         <v>140</v>
       </c>
@@ -7411,14 +7486,14 @@
       <c r="D188" t="s">
         <v>264</v>
       </c>
-      <c r="H188" t="s">
+      <c r="I188" t="s">
         <v>240</v>
       </c>
-      <c r="I188" t="s">
+      <c r="J188" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="189" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B189" t="s">
         <v>154</v>
       </c>
@@ -7428,14 +7503,14 @@
       <c r="D189" t="s">
         <v>264</v>
       </c>
-      <c r="H189" t="s">
+      <c r="I189" t="s">
         <v>240</v>
       </c>
-      <c r="I189" t="s">
+      <c r="J189" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="190" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B190" t="s">
         <v>175</v>
       </c>
@@ -7445,14 +7520,14 @@
       <c r="D190" t="s">
         <v>264</v>
       </c>
-      <c r="H190" t="s">
+      <c r="I190" t="s">
         <v>242</v>
       </c>
-      <c r="I190" t="s">
+      <c r="J190" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="191" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
         <v>143</v>
       </c>
@@ -7462,14 +7537,14 @@
       <c r="D191" t="s">
         <v>264</v>
       </c>
-      <c r="H191" t="s">
+      <c r="I191" t="s">
         <v>240</v>
       </c>
-      <c r="I191" t="s">
+      <c r="J191" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="192" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B192" t="s">
         <v>83</v>
       </c>
@@ -7479,14 +7554,14 @@
       <c r="D192" t="s">
         <v>264</v>
       </c>
-      <c r="H192" t="s">
+      <c r="I192" t="s">
         <v>252</v>
       </c>
-      <c r="I192" t="s">
+      <c r="J192" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="193" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B193" t="s">
         <v>86</v>
       </c>
@@ -7496,14 +7571,14 @@
       <c r="D193" t="s">
         <v>264</v>
       </c>
-      <c r="H193" t="s">
+      <c r="I193" t="s">
         <v>240</v>
       </c>
-      <c r="I193" t="s">
+      <c r="J193" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="194" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B194" t="s">
         <v>145</v>
       </c>
@@ -7513,14 +7588,14 @@
       <c r="D194" t="s">
         <v>264</v>
       </c>
-      <c r="H194" t="s">
+      <c r="I194" t="s">
         <v>240</v>
       </c>
-      <c r="I194" t="s">
+      <c r="J194" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="195" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B195" t="s">
         <v>151</v>
       </c>
@@ -7533,14 +7608,14 @@
       <c r="F195" t="b">
         <v>0</v>
       </c>
-      <c r="H195" t="s">
+      <c r="I195" t="s">
         <v>240</v>
       </c>
-      <c r="I195" t="s">
+      <c r="J195" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="196" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B196" t="s">
         <v>48</v>
       </c>
@@ -7550,17 +7625,17 @@
       <c r="D196" t="s">
         <v>264</v>
       </c>
-      <c r="F196" t="b">
-        <v>0</v>
-      </c>
-      <c r="H196" t="s">
+      <c r="G196" t="b">
+        <v>1</v>
+      </c>
+      <c r="I196" t="s">
         <v>248</v>
       </c>
-      <c r="I196" t="s">
+      <c r="J196" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="197" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B197" t="s">
         <v>111</v>
       </c>
@@ -7570,14 +7645,14 @@
       <c r="D197" t="s">
         <v>264</v>
       </c>
-      <c r="H197" t="s">
+      <c r="I197" t="s">
         <v>240</v>
       </c>
-      <c r="I197" t="s">
+      <c r="J197" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="198" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B198" t="s">
         <v>93</v>
       </c>
@@ -7587,14 +7662,14 @@
       <c r="D198" t="s">
         <v>264</v>
       </c>
-      <c r="H198" t="s">
+      <c r="I198" t="s">
         <v>240</v>
       </c>
-      <c r="I198" t="s">
+      <c r="J198" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="199" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B199" t="s">
         <v>150</v>
       </c>
@@ -7604,14 +7679,14 @@
       <c r="D199" t="s">
         <v>264</v>
       </c>
-      <c r="H199" t="s">
+      <c r="I199" t="s">
         <v>248</v>
       </c>
-      <c r="I199" t="s">
+      <c r="J199" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="200" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B200" t="s">
         <v>171</v>
       </c>
@@ -7624,14 +7699,14 @@
       <c r="F200" t="b">
         <v>0</v>
       </c>
-      <c r="H200" t="s">
+      <c r="I200" t="s">
         <v>258</v>
       </c>
-      <c r="I200" t="s">
+      <c r="J200" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="201" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B201" t="s">
         <v>100</v>
       </c>
@@ -7641,14 +7716,14 @@
       <c r="D201" t="s">
         <v>264</v>
       </c>
-      <c r="H201" t="s">
+      <c r="I201" t="s">
         <v>240</v>
       </c>
-      <c r="I201" t="s">
+      <c r="J201" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="202" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B202" t="s">
         <v>165</v>
       </c>
@@ -7658,14 +7733,14 @@
       <c r="D202" t="s">
         <v>264</v>
       </c>
-      <c r="H202" t="s">
+      <c r="I202" t="s">
         <v>242</v>
       </c>
-      <c r="I202" t="s">
+      <c r="J202" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="203" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B203" t="s">
         <v>113</v>
       </c>
@@ -7675,14 +7750,14 @@
       <c r="D203" t="s">
         <v>264</v>
       </c>
-      <c r="H203" t="s">
+      <c r="I203" t="s">
         <v>240</v>
       </c>
-      <c r="I203" t="s">
+      <c r="J203" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="204" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B204" t="s">
         <v>75</v>
       </c>
@@ -7692,14 +7767,14 @@
       <c r="D204" t="s">
         <v>264</v>
       </c>
-      <c r="H204" t="s">
+      <c r="I204" t="s">
         <v>242</v>
       </c>
-      <c r="I204" t="s">
+      <c r="J204" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="205" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B205" t="s">
         <v>31</v>
       </c>
@@ -7709,14 +7784,14 @@
       <c r="D205" t="s">
         <v>264</v>
       </c>
-      <c r="H205" t="s">
+      <c r="I205" t="s">
         <v>240</v>
       </c>
-      <c r="I205" t="s">
+      <c r="J205" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="206" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B206" t="s">
         <v>204</v>
       </c>
@@ -7733,7 +7808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B207" t="s">
         <v>213</v>
       </c>
@@ -7749,11 +7824,11 @@
       <c r="F207" t="b">
         <v>0</v>
       </c>
-      <c r="J207" t="s">
+      <c r="K207" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="208" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B208" t="s">
         <v>184</v>
       </c>
@@ -7770,7 +7845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B209" t="s">
         <v>215</v>
       </c>
@@ -7787,7 +7862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B210" t="s">
         <v>71</v>
       </c>
@@ -7804,7 +7879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B211" t="s">
         <v>202</v>
       </c>
@@ -7821,7 +7896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B212" t="s">
         <v>220</v>
       </c>
@@ -7838,7 +7913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B213" t="s">
         <v>211</v>
       </c>
@@ -7855,7 +7930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B214" t="s">
         <v>214</v>
       </c>
@@ -7872,7 +7947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B215" t="s">
         <v>198</v>
       </c>
@@ -7889,7 +7964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B216" t="s">
         <v>228</v>
       </c>
@@ -7906,7 +7981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B217" t="s">
         <v>180</v>
       </c>
@@ -7923,7 +7998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B218" t="s">
         <v>189</v>
       </c>
@@ -7940,7 +8015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B219" t="s">
         <v>188</v>
       </c>
@@ -7957,7 +8032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B220" t="s">
         <v>199</v>
       </c>
@@ -7974,7 +8049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B221" t="s">
         <v>195</v>
       </c>
@@ -7991,7 +8066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B222" t="s">
         <v>201</v>
       </c>
@@ -8008,7 +8083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B223" t="s">
         <v>69</v>
       </c>
@@ -8018,17 +8093,20 @@
       <c r="D223" t="s">
         <v>266</v>
       </c>
-      <c r="H223" t="s">
+      <c r="G223" t="b">
+        <v>1</v>
+      </c>
+      <c r="I223" t="s">
         <v>240</v>
       </c>
-      <c r="I223" t="s">
+      <c r="J223" t="s">
         <v>239</v>
       </c>
-      <c r="J223" t="s">
+      <c r="K223" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="224" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B224" t="s">
         <v>197</v>
       </c>
@@ -8197,10 +8275,10 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:J238">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K238">
     <sortCondition ref="C2:C238"/>
     <sortCondition ref="D2:D238"/>
-    <sortCondition ref="I2:I238"/>
+    <sortCondition ref="J2:J238"/>
     <sortCondition ref="B2:B238"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8211,7 +8289,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79DCE686-8F0B-4BA6-9AD3-B6DCBE0850B0}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8535,7 +8615,7 @@
         <v>28</v>
       </c>
       <c r="P17">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -8560,6 +8640,9 @@
       </c>
       <c r="H18">
         <v>23</v>
+      </c>
+      <c r="I18" t="s">
+        <v>284</v>
       </c>
       <c r="M18" t="s">
         <v>266</v>

</xml_diff>